<commit_message>
Update Excel table with strings to be translated
</commit_message>
<xml_diff>
--- a/SignalAnalysis/localization/Remaining strings translation.xlsx
+++ b/SignalAnalysis/localization/Remaining strings translation.xlsx
@@ -193,7 +193,7 @@
       </x:c>
       <x:c r="D2" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">In plot derivative</x:t>
         </x:is>
       </x:c>
       <x:c r="E2" t="inlineStr">
@@ -315,7 +315,7 @@
       </x:c>
       <x:c r="D3" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">In plot derivative</x:t>
         </x:is>
       </x:c>
       <x:c r="E3" t="inlineStr">
@@ -432,17 +432,17 @@
       </x:c>
       <x:c r="C4" s="1" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">strPlotDerivativeYLabel</x:t>
+          <x:t xml:space="preserve">strPlotDerivativeYLabel1</x:t>
         </x:is>
       </x:c>
       <x:c r="D4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">In plot derivative</x:t>
         </x:is>
       </x:c>
       <x:c r="E4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Amplitude / seconds</x:t>
+          <x:t xml:space="preserve">Amplitude / sec</x:t>
         </x:is>
       </x:c>
       <x:c r="F4" t="inlineStr">
@@ -472,7 +472,7 @@
       </x:c>
       <x:c r="K4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Amplitude / seconds</x:t>
+          <x:t xml:space="preserve">Amplitude / sec</x:t>
         </x:is>
       </x:c>
       <x:c r="L4" t="inlineStr">
@@ -532,7 +532,7 @@
       </x:c>
       <x:c r="W4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Amplitud / segundos</x:t>
+          <x:t xml:space="preserve">Amplitud / seg</x:t>
         </x:is>
       </x:c>
       <x:c r="X4" t="inlineStr">
@@ -559,7 +559,7 @@
       </x:c>
       <x:c r="D5" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Column text header in exported files</x:t>
         </x:is>
       </x:c>
       <x:c r="E5" t="inlineStr">
@@ -681,7 +681,7 @@
       </x:c>
       <x:c r="D6" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">Tab text in "settings" form</x:t>
         </x:is>
       </x:c>
       <x:c r="E6" t="inlineStr">
@@ -803,7 +803,7 @@
       </x:c>
       <x:c r="D7" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">In "settings" form</x:t>
         </x:is>
       </x:c>
       <x:c r="E7" t="inlineStr">
@@ -925,7 +925,7 @@
       </x:c>
       <x:c r="D8" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">In "settings" form</x:t>
         </x:is>
       </x:c>
       <x:c r="E8" t="inlineStr">
@@ -1047,7 +1047,7 @@
       </x:c>
       <x:c r="D9" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">In "settings" form</x:t>
         </x:is>
       </x:c>
       <x:c r="E9" t="inlineStr">
@@ -1169,7 +1169,7 @@
       </x:c>
       <x:c r="D10" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">In "settings" form, mathematical name</x:t>
         </x:is>
       </x:c>
       <x:c r="E10" t="inlineStr">
@@ -1291,7 +1291,7 @@
       </x:c>
       <x:c r="D11" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">In "settings" form, mathematical name</x:t>
         </x:is>
       </x:c>
       <x:c r="E11" t="inlineStr">
@@ -1413,7 +1413,7 @@
       </x:c>
       <x:c r="D12" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">In "settings" form, mathematical name</x:t>
         </x:is>
       </x:c>
       <x:c r="E12" t="inlineStr">
@@ -1508,7 +1508,7 @@
       </x:c>
       <x:c r="W12" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Diferencia central de 3 puntos</x:t>
+          <x:t xml:space="preserve">Diferencias centrales de 3 puntos</x:t>
         </x:is>
       </x:c>
       <x:c r="X12" t="inlineStr">
@@ -1535,7 +1535,7 @@
       </x:c>
       <x:c r="D13" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve"/>
+          <x:t xml:space="preserve">In "settings" form, mathematical name</x:t>
         </x:is>
       </x:c>
       <x:c r="E13" t="inlineStr">
@@ -1630,10 +1630,254 @@
       </x:c>
       <x:c r="W13" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">Diferencia central de 5 puntos</x:t>
+          <x:t xml:space="preserve">Diferencias centrales de 5 puntos</x:t>
         </x:is>
       </x:c>
       <x:c r="X13" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c r="A14" s="1" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">SignalAnalysis</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B14" s="1" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">localization\strings</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C14" s="1" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">strPlotDerivativeYLabel2</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">In plot derivative</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Amplitude</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="G14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="H14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="I14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="J14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="K14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Amplitude</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="L14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="M14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="N14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="O14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="P14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="Q14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="R14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="S14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="T14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="U14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="V14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="W14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Amplitud</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="X14" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c r="A15" s="1" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">SignalAnalysis</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B15" s="1" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">localization\strings</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C15" s="1" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">strStatusTipDerivative</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="E15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Numerical differentiation</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="G15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="H15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="I15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="J15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="K15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Numerical differentiation</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="L15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="M15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="N15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="O15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="P15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="Q15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="R15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="S15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="T15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="U15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="V15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve"/>
+        </x:is>
+      </x:c>
+      <x:c r="W15" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Derivada numérica</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="X15" t="inlineStr">
         <x:is>
           <x:t xml:space="preserve"/>
         </x:is>

</xml_diff>